<commit_message>
Start 2nd version of writing
</commit_message>
<xml_diff>
--- a/FencingVis/Public/data/men_final_v2.xlsx
+++ b/FencingVis/Public/data/men_final_v2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="53">
   <si>
     <t>time</t>
   </si>
@@ -166,10 +166,20 @@
   </si>
   <si>
     <t>parry_pos1</t>
+  </si>
+  <si>
+    <t>parry_pos2</t>
+  </si>
+  <si>
+    <t>bf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>parry_pos2</t>
+    <t>cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -504,8 +514,8 @@
   <dimension ref="A1:O1860"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A777" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G814" sqref="G814"/>
+      <pane ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B316" sqref="B316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2250,24 +2260,21 @@
       <c r="A248" s="2">
         <v>0.21481481481481482</v>
       </c>
-      <c r="B248" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C248" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="2">
         <v>0.21482638888888891</v>
       </c>
+      <c r="C249" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
         <v>0.21483796296296298</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>12</v>
@@ -2277,6 +2284,9 @@
       <c r="A251" s="2">
         <v>0.21484953703703702</v>
       </c>
+      <c r="B251" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
@@ -2394,7 +2404,7 @@
         <v>0.21541666666666667</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
@@ -2420,7 +2430,7 @@
         <v>0.21546296296296297</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>12</v>
@@ -2564,7 +2574,7 @@
         <v>0.21608796296296295</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
@@ -2669,7 +2679,7 @@
         <v>0.21629629629629629</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
@@ -4911,7 +4921,7 @@
         <v>0.28275462962962966</v>
       </c>
       <c r="B666" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.2">
@@ -4955,7 +4965,7 @@
         <v>0.28283564814814816</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.2">
@@ -5159,7 +5169,7 @@
         <v>0.28356481481481483</v>
       </c>
       <c r="B706" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="707" spans="1:3" x14ac:dyDescent="0.2">
@@ -5207,7 +5217,7 @@
         <v>0.28366898148148151</v>
       </c>
       <c r="B715" s="1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C715" s="1" t="s">
         <v>13</v>
@@ -11383,7 +11393,7 @@
         <v>15</v>
       </c>
       <c r="C1641" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="1642" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>